<commit_message>
Week 3 Commit 6
</commit_message>
<xml_diff>
--- a/docs/BagUnitTest.xlsx
+++ b/docs/BagUnitTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kayle\OneDrive\Documents\CS372\week1\cs372.hurst\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A24C296C-1F28-48A0-A747-28A099AACD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CC5E85-6B02-4470-B4B0-FF2ED8179EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{47BF89DF-1999-449D-99E8-5FB82A9EB84A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>:</t>
   </si>
@@ -75,52 +75,55 @@
     <t>integers 0-9</t>
   </si>
   <si>
-    <t>bag contains integers 0-9</t>
-  </si>
-  <si>
-    <t>Test ID: Print Behavior</t>
-  </si>
-  <si>
-    <t>aBagOfIntegers</t>
-  </si>
-  <si>
-    <t>prints to screen 0-9</t>
-  </si>
-  <si>
-    <t>Test ID: Remove Behavior</t>
-  </si>
-  <si>
-    <t>aBagOfIntegers.remove(9);</t>
-  </si>
-  <si>
-    <t>aBagOfIntegers contains 0-8;</t>
-  </si>
-  <si>
     <t>Test ID: Size Behavior</t>
   </si>
   <si>
     <t>Input Data:</t>
   </si>
   <si>
-    <t>aBagOfIntegers contains 9 integers</t>
-  </si>
-  <si>
     <t>aBagOfIntegers.size();</t>
   </si>
   <si>
-    <t>size should be 9</t>
-  </si>
-  <si>
-    <t>Test ID: Count Behavior</t>
-  </si>
-  <si>
-    <t>aBagOfIntegers.count();</t>
-  </si>
-  <si>
-    <t>aBagOfIntegers contains 3 integers</t>
-  </si>
-  <si>
-    <t>print 3 to the screen</t>
+    <t>aBagOfIntegers contains 10 integers</t>
+  </si>
+  <si>
+    <t>"There are now 10 items in your bag."</t>
+  </si>
+  <si>
+    <t>Test ID: Count Behavior w/ duplicate</t>
+  </si>
+  <si>
+    <t>Test ID: Count Behavior w/o duplicate</t>
+  </si>
+  <si>
+    <t>Test ID: Count Behavior w/ no instance</t>
+  </si>
+  <si>
+    <t>added another 9 to the bag</t>
+  </si>
+  <si>
+    <t>aBagOfIntegers.count(9);</t>
+  </si>
+  <si>
+    <t>aBagOfIntegers.count(1);</t>
+  </si>
+  <si>
+    <t>aBagOfIntegers.count(25);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is only one </t>
+  </si>
+  <si>
+    <t>there is none</t>
+  </si>
+  <si>
+    <t>"The number '9' is in this list 2 times."</t>
+  </si>
+  <si>
+    <t>"The number '1' is in this list 1 times."</t>
+  </si>
+  <si>
+    <t>"The number '25' is in this list 0 times."</t>
   </si>
 </sst>
 </file>
@@ -509,7 +512,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +610,7 @@
         <v>13</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -615,12 +618,12 @@
         <v>14</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -628,12 +631,12 @@
         <v>11</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>18</v>
@@ -644,7 +647,7 @@
         <v>13</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -652,12 +655,12 @@
         <v>14</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -665,15 +668,15 @@
         <v>11</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -681,7 +684,7 @@
         <v>13</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -689,12 +692,12 @@
         <v>14</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -702,12 +705,12 @@
         <v>11</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>26</v>
@@ -718,7 +721,7 @@
         <v>13</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -731,7 +734,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -739,23 +742,23 @@
         <v>11</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>